<commit_message>
copying changes from MBT rep into here
</commit_message>
<xml_diff>
--- a/AOS_ADDTOCART_OCT_OR/Default.xlsx
+++ b/AOS_ADDTOCART_OCT_OR/Default.xlsx
@@ -473,12 +473,12 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.1"/>
+  <sheetFormatPr defaultRowHeight="14.95"/>
   <cols>
     <col min="1" max="16384" width="8.8984375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="14.95" customFormat="1"/>
+    <row r="1" customFormat="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>